<commit_message>
Adding new results to the spreadsheet
</commit_message>
<xml_diff>
--- a/documents/analysis/BFPAnalysis.xlsx
+++ b/documents/analysis/BFPAnalysis.xlsx
@@ -586,7 +586,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
   <si>
     <t>nodes = 5</t>
   </si>
@@ -812,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -909,6 +909,21 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -930,24 +945,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1470,8 +1472,8 @@
       <c r="J9" s="17">
         <v>20</v>
       </c>
-      <c r="K9" s="62">
-        <f>1/(C9*D9)</f>
+      <c r="K9" s="55">
+        <f t="shared" ref="K9:K17" si="0">1/(C9*D9)</f>
         <v>0.05</v>
       </c>
     </row>
@@ -1500,8 +1502,8 @@
       <c r="J10" s="17">
         <v>20</v>
       </c>
-      <c r="K10" s="62">
-        <f>1/(C10*D10)</f>
+      <c r="K10" s="55">
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -1530,8 +1532,8 @@
       <c r="J11" s="17">
         <v>20</v>
       </c>
-      <c r="K11" s="62">
-        <f>1/(C11*D11)</f>
+      <c r="K11" s="55">
+        <f t="shared" si="0"/>
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
@@ -1556,8 +1558,8 @@
       <c r="J12" s="32">
         <v>20</v>
       </c>
-      <c r="K12" s="62">
-        <f>1/(C12*D12)</f>
+      <c r="K12" s="55">
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
@@ -1578,8 +1580,8 @@
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="32"/>
-      <c r="K13" s="62">
-        <f>1/(C13*D13)</f>
+      <c r="K13" s="55">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
@@ -1600,8 +1602,8 @@
       <c r="H14" s="32"/>
       <c r="I14" s="30"/>
       <c r="J14" s="32"/>
-      <c r="K14" s="62">
-        <f>1/(C14*D14)</f>
+      <c r="K14" s="55">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
@@ -1620,8 +1622,8 @@
       <c r="H15" s="32"/>
       <c r="I15" s="30"/>
       <c r="J15" s="32"/>
-      <c r="K15" s="62">
-        <f>1/(C15*D15)</f>
+      <c r="K15" s="55">
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
@@ -1642,8 +1644,8 @@
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
       <c r="J16" s="32"/>
-      <c r="K16" s="62">
-        <f>1/(C16*D16)</f>
+      <c r="K16" s="55">
+        <f t="shared" si="0"/>
         <v>2.2222222222222222E-3</v>
       </c>
     </row>
@@ -1657,21 +1659,21 @@
       <c r="E17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="64">
+      <c r="F17" s="57">
         <v>7.3618181818180002</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="63">
-        <f>1/(C17*D17)</f>
+      <c r="K17" s="56">
+        <f t="shared" si="0"/>
         <v>1.8181818181818182E-3</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C18" s="32"/>
-      <c r="D18" s="61"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="7"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
@@ -1694,7 +1696,7 @@
   <dimension ref="B2:S33"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1709,28 +1711,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="O2" s="54" t="s">
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="O2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="11"/>
@@ -1782,7 +1784,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="67" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="22">
@@ -1833,7 +1835,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="59"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="20">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -1882,7 +1884,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B6" s="59"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="20">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1931,7 +1933,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="59"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="20">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -1980,7 +1982,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="59"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="20">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -2029,7 +2031,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="59"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="20">
         <v>4.4999999999999997E-3</v>
       </c>
@@ -2076,7 +2078,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="59"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="20">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -2119,7 +2121,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="60"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="21"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24">
@@ -2284,7 +2286,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="67" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="46">
@@ -2335,7 +2337,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B16" s="59"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="47">
         <v>3.712E-3</v>
       </c>
@@ -2384,7 +2386,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B17" s="59"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="47">
         <v>3.6310000000000001E-3</v>
       </c>
@@ -2433,7 +2435,7 @@
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="59"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="47">
         <v>3.5200000000000001E-3</v>
       </c>
@@ -2482,7 +2484,7 @@
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B19" s="59"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="47">
         <v>6.0010000000000003E-3</v>
       </c>
@@ -2531,7 +2533,7 @@
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B20" s="59"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="47">
         <v>3.6089999999999998E-3</v>
       </c>
@@ -2578,7 +2580,7 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="59"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="47">
         <v>3.7139999999999999E-3</v>
       </c>
@@ -2621,7 +2623,7 @@
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="60"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="48"/>
       <c r="D22" s="48"/>
       <c r="E22" s="48">
@@ -2717,27 +2719,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:19" s="68" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
-      <c r="M24" s="67"/>
-      <c r="O24" s="69"/>
-      <c r="P24" s="69"/>
-      <c r="Q24" s="69"/>
-      <c r="R24" s="69"/>
-      <c r="S24" s="69"/>
+    <row r="24" spans="2:19" s="60" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="61"/>
+      <c r="S24" s="61"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="62" t="s">
         <v>28</v>
       </c>
       <c r="C25">
@@ -2745,46 +2747,46 @@
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B26" s="70"/>
+      <c r="B26" s="62"/>
       <c r="C26">
         <v>2.25</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="70"/>
+      <c r="B27" s="62"/>
       <c r="C27">
         <v>1.35</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B28" s="70"/>
+      <c r="B28" s="62"/>
       <c r="C28">
         <v>1.35</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B29" s="70"/>
+      <c r="B29" s="62"/>
       <c r="C29">
         <v>1.25</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B30" s="70"/>
+      <c r="B30" s="62"/>
       <c r="C30">
         <v>1.45</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B31" s="70"/>
+      <c r="B31" s="62"/>
       <c r="C31">
         <v>1.35</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B32" s="70"/>
+      <c r="B32" s="62"/>
     </row>
     <row r="33" spans="2:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="58" t="s">
         <v>27</v>
       </c>
       <c r="C33">
@@ -2809,7 +2811,7 @@
   <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2835,7 +2837,7 @@
       <c r="G5" s="27"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="67" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="22">
@@ -2849,7 +2851,7 @@
       <c r="G6" s="22"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="59"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="20">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -2861,7 +2863,7 @@
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="59"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="20">
         <v>5.4000000000000003E-3</v>
       </c>
@@ -2873,7 +2875,7 @@
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="59"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="20">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2885,7 +2887,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="59"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="20">
         <v>2E-3</v>
       </c>
@@ -2897,7 +2899,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="59"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="20">
         <v>3.8E-3</v>
       </c>
@@ -2909,7 +2911,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="59"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="20">
         <v>5.5999999999999999E-3</v>
       </c>
@@ -2921,7 +2923,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="60"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="21"/>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
@@ -2972,13 +2974,13 @@
       <c r="G16" s="27"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="71">
         <v>3.5760000000000002E-3</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="71">
         <v>8.8310000000000003E-3</v>
       </c>
       <c r="E17" s="46"/>
@@ -2986,11 +2988,11 @@
       <c r="G17" s="46"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="59"/>
-      <c r="C18" s="20">
+      <c r="B18" s="68"/>
+      <c r="C18" s="72">
         <v>3.6180000000000001E-3</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="72">
         <v>6.0219999999999996E-3</v>
       </c>
       <c r="E18" s="47"/>
@@ -2998,11 +3000,11 @@
       <c r="G18" s="47"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="59"/>
-      <c r="C19" s="20">
+      <c r="B19" s="68"/>
+      <c r="C19" s="72">
         <v>5.8820000000000001E-3</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="72">
         <v>5.9160000000000003E-3</v>
       </c>
       <c r="E19" s="47"/>
@@ -3010,11 +3012,11 @@
       <c r="G19" s="47"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="59"/>
-      <c r="C20" s="20">
+      <c r="B20" s="68"/>
+      <c r="C20" s="72">
         <v>3.4480000000000001E-3</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="72">
         <v>8.7889999999999999E-3</v>
       </c>
       <c r="E20" s="47"/>
@@ -3022,11 +3024,11 @@
       <c r="G20" s="47"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="59"/>
-      <c r="C21" s="20">
+      <c r="B21" s="68"/>
+      <c r="C21" s="72">
         <v>3.7139999999999999E-3</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="72">
         <v>5.8650000000000004E-3</v>
       </c>
       <c r="E21" s="47"/>
@@ -3034,11 +3036,11 @@
       <c r="G21" s="47"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="59"/>
-      <c r="C22" s="47">
+      <c r="B22" s="68"/>
+      <c r="C22" s="72">
         <v>3.5799999999999998E-3</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="72">
         <v>5.9540000000000001E-3</v>
       </c>
       <c r="E22" s="47"/>
@@ -3046,11 +3048,11 @@
       <c r="G22" s="47"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="59"/>
-      <c r="C23" s="47">
+      <c r="B23" s="68"/>
+      <c r="C23" s="72">
         <v>5.8399999999999997E-3</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="72">
         <v>8.8050000000000003E-3</v>
       </c>
       <c r="E23" s="47"/>
@@ -3058,7 +3060,7 @@
       <c r="G23" s="47"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="60"/>
+      <c r="B24" s="69"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
@@ -3089,7 +3091,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="70" t="s">
         <v>28</v>
       </c>
       <c r="C27">
@@ -3100,7 +3102,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="66"/>
+      <c r="B28" s="70"/>
       <c r="C28">
         <v>1.26</v>
       </c>
@@ -3109,7 +3111,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="66"/>
+      <c r="B29" s="70"/>
       <c r="C29">
         <v>1.6</v>
       </c>
@@ -3118,7 +3120,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="66"/>
+      <c r="B30" s="70"/>
       <c r="C30">
         <v>1.4</v>
       </c>
@@ -3127,7 +3129,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="66"/>
+      <c r="B31" s="70"/>
       <c r="C31">
         <v>2.2000000000000002</v>
       </c>
@@ -3136,7 +3138,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="66"/>
+      <c r="B32" s="70"/>
       <c r="C32">
         <v>1.4</v>
       </c>
@@ -3145,7 +3147,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="66"/>
+      <c r="B33" s="70"/>
       <c r="C33">
         <v>1.58</v>
       </c>
@@ -3154,7 +3156,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="58" t="s">
         <v>27</v>
       </c>
       <c r="C34">
@@ -3178,8 +3180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3198,114 +3200,116 @@
         <v>13</v>
       </c>
       <c r="D4" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="F4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="67" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="22">
         <v>1.5E-3</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="22"/>
+      <c r="E5" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="E5" s="22">
+      <c r="F5" s="22">
         <v>1.14E-2</v>
       </c>
-      <c r="F5" s="22"/>
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="59"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="20">
         <v>1.5E-3</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E6" s="20">
+      <c r="F6" s="20">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="F6" s="20"/>
       <c r="G6" s="20"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="59"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20">
         <v>1.23E-2</v>
       </c>
-      <c r="E7" s="20">
+      <c r="F7" s="20">
         <v>1.12E-2</v>
       </c>
-      <c r="F7" s="20"/>
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="59"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="20"/>
+      <c r="E8" s="20">
         <v>9.5999999999999992E-3</v>
       </c>
-      <c r="E8" s="20">
+      <c r="F8" s="20">
         <v>1.29E-2</v>
       </c>
-      <c r="F8" s="20"/>
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="59"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="20">
         <v>1.4E-3</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="20"/>
+      <c r="E9" s="20">
         <v>1.09E-2</v>
       </c>
-      <c r="E9" s="20">
+      <c r="F9" s="20">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="59"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="20"/>
-      <c r="D10" s="20">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20">
         <v>1.21E-2</v>
       </c>
-      <c r="E10" s="20">
+      <c r="F10" s="20">
         <v>1.06E-2</v>
       </c>
-      <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="59"/>
+      <c r="B11" s="68"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="20">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="E11" s="23"/>
       <c r="F11" s="23"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="60"/>
+      <c r="B12" s="69"/>
       <c r="C12" s="21"/>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="21"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
@@ -3316,15 +3320,15 @@
       </c>
       <c r="D13" s="25">
         <f>MAX(D5:D12)</f>
-        <v>1.3100000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="25">
         <f>MAX(E5:E12)</f>
-        <v>1.2999999999999999E-2</v>
+        <v>1.3100000000000001E-2</v>
       </c>
       <c r="F13" s="25">
         <f>MAX(F5:F12)</f>
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G13" s="25">
         <f>MAX(G5:G12)</f>
@@ -3356,7 +3360,7 @@
       <c r="G15" s="27"/>
     </row>
     <row r="16" spans="2:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="67" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="22">
@@ -3372,7 +3376,7 @@
       <c r="G16" s="46"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="59"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -3386,7 +3390,7 @@
       <c r="G17" s="47"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="59"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="20">
         <v>1.6000000000000001E-3</v>
       </c>
@@ -3400,7 +3404,7 @@
       <c r="G18" s="47"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="59"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="20">
         <v>1.4E-3</v>
       </c>
@@ -3414,7 +3418,7 @@
       <c r="G19" s="47"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="59"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
@@ -3428,7 +3432,7 @@
       <c r="G20" s="47"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="59"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
       <c r="E21" s="47">
@@ -3440,7 +3444,7 @@
       <c r="G21" s="47"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="59"/>
+      <c r="B22" s="68"/>
       <c r="C22" s="47"/>
       <c r="D22" s="47"/>
       <c r="E22" s="47">
@@ -3450,7 +3454,7 @@
       <c r="G22" s="47"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="60"/>
+      <c r="B23" s="69"/>
       <c r="C23" s="48"/>
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
@@ -3481,7 +3485,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="70" t="s">
         <v>28</v>
       </c>
       <c r="E26">
@@ -3492,7 +3496,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="66"/>
+      <c r="B27" s="70"/>
       <c r="E27">
         <v>1.2533300000000001</v>
       </c>
@@ -3501,7 +3505,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="66"/>
+      <c r="B28" s="70"/>
       <c r="E28">
         <v>1.28</v>
       </c>
@@ -3510,7 +3514,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="66"/>
+      <c r="B29" s="70"/>
       <c r="E29">
         <v>1.22444</v>
       </c>
@@ -3519,7 +3523,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="66"/>
+      <c r="B30" s="70"/>
       <c r="E30">
         <v>1.26</v>
       </c>
@@ -3528,7 +3532,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="66"/>
+      <c r="B31" s="70"/>
       <c r="E31">
         <v>1.2888900000000001</v>
       </c>
@@ -3537,10 +3541,10 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="66"/>
+      <c r="B32" s="70"/>
     </row>
     <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="65" t="s">
+      <c r="B33" s="58" t="s">
         <v>27</v>
       </c>
       <c r="E33">
@@ -3588,13 +3592,13 @@
       </c>
     </row>
     <row r="2" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C3" s="11"/>
@@ -3615,7 +3619,7 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="67" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="22">
@@ -3635,7 +3639,7 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C5" s="59"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="20">
         <v>1.5E-3</v>
       </c>
@@ -3653,7 +3657,7 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C6" s="59"/>
+      <c r="C6" s="68"/>
       <c r="D6" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
@@ -3671,7 +3675,7 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="59"/>
+      <c r="C7" s="68"/>
       <c r="D7" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -3689,7 +3693,7 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C8" s="59"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="20">
         <v>1.4E-3</v>
       </c>
@@ -3707,7 +3711,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="59"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23">
         <v>2.2000000000000001E-3</v>
@@ -3723,7 +3727,7 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="59"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="20"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23">
@@ -3735,7 +3739,7 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="60"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="21"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24">
@@ -3788,7 +3792,7 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="67" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="22">
@@ -3808,7 +3812,7 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="59"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -3826,7 +3830,7 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="59"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="20">
         <v>1.6000000000000001E-3</v>
       </c>
@@ -3844,7 +3848,7 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C17" s="59"/>
+      <c r="C17" s="68"/>
       <c r="D17" s="20">
         <v>1.4E-3</v>
       </c>
@@ -3862,7 +3866,7 @@
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C18" s="59"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
@@ -3880,7 +3884,7 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C19" s="59"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23">
         <v>3.7829999999999999E-3</v>
@@ -3896,7 +3900,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C20" s="59"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="20"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23">
@@ -3908,7 +3912,7 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C21" s="60"/>
+      <c r="C21" s="69"/>
       <c r="D21" s="21"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24">

</xml_diff>

<commit_message>
Updating files for merging
</commit_message>
<xml_diff>
--- a/documents/analysis/BFPAnalysis.xlsx
+++ b/documents/analysis/BFPAnalysis.xlsx
@@ -171,7 +171,6 @@
           </rPr>
           <t xml:space="preserve">
 149.46 seconds
-# scenarios 2000
 p(x) = 0.0089</t>
         </r>
       </text>
@@ -448,7 +447,6 @@
           </rPr>
           <t xml:space="preserve">
 52395.82 seconds
-# scenarios 5000
 p(x)=0.003783
 </t>
         </r>
@@ -526,8 +524,32 @@
           </rPr>
           <t xml:space="preserve">
 3407.19 seconds
-# scenarios = 10000
 p(x) = 0.0022</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+9445.40 seconds
+p(x)=0.01233</t>
         </r>
       </text>
     </comment>
@@ -539,7 +561,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -548,11 +570,11 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-9445.40 seconds
-p(x)=0.01233</t>
+15240.07 seconds
+p(x)=0.01227</t>
         </r>
       </text>
     </comment>
@@ -564,6 +586,156 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+86.85 seconds
+p(x)=0.001726</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+145.85 seconds
+p(x)=0.003814</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+435.14 seconds
+p(x)=0.004597</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+312.02 seconds
+p(x)=0.100237</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+3.26 seconds
+p(x)=0.250675</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+233.05 seconds
+p(x)=0.001661</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t>Author:</t>
@@ -573,11 +745,61 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+54.51 seconds
+p(x) = 0.012</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+206.91 seconds
+p(x)= 0.0122</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">
-15240.07 seconds
-p(x)=0.01227</t>
+1533.54 seconds
+p(x) = 0.012</t>
         </r>
       </text>
     </comment>
@@ -586,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="32">
   <si>
     <t>nodes = 5</t>
   </si>
@@ -692,6 +914,9 @@
   </si>
   <si>
     <t>ϵ=0.02</t>
+  </si>
+  <si>
+    <t>BFPIS</t>
   </si>
 </sst>
 </file>
@@ -812,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -870,13 +1095,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -921,6 +1140,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,8 +1187,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1254,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:K19"/>
+  <dimension ref="C1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1317,7 +1554,7 @@
       <c r="D4" s="27">
         <v>0.01</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="37" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="27">
@@ -1340,110 +1577,110 @@
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C5" s="29"/>
-      <c r="D5" s="29">
+      <c r="C5" s="63"/>
+      <c r="D5" s="63">
         <v>0.01</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="63">
         <v>10</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="63">
         <v>15</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="63">
         <v>15</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="63">
         <v>20</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="63">
         <v>30</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="63" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C6" s="29"/>
-      <c r="D6" s="29">
+      <c r="C6" s="63"/>
+      <c r="D6" s="63">
         <v>0.01</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="63">
         <v>8</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="63">
         <v>16</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="63">
         <v>16</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="63">
         <v>16</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="63">
         <v>24</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="63" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C7" s="29"/>
-      <c r="D7" s="29">
+      <c r="C7" s="63"/>
+      <c r="D7" s="63">
         <v>0.01</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="63">
         <v>20</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="63">
         <v>20</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="63">
         <v>20</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="63">
         <v>20</v>
       </c>
-      <c r="J7" s="29">
+      <c r="J7" s="63">
         <v>20</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="K7" s="63" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C8" s="29"/>
-      <c r="D8" s="29">
+      <c r="C8" s="66"/>
+      <c r="D8" s="66">
         <v>0.01</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="66">
         <v>7</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="66">
         <v>11</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="66">
         <v>13</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="66">
         <v>16</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="66">
         <v>20</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="66" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1457,7 +1694,7 @@
       <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>10.5</v>
       </c>
       <c r="G9" s="17">
@@ -1472,8 +1709,8 @@
       <c r="J9" s="17">
         <v>20</v>
       </c>
-      <c r="K9" s="55">
-        <f t="shared" ref="K9:K17" si="0">1/(C9*D9)</f>
+      <c r="K9" s="53">
+        <f t="shared" ref="K9:K18" si="0">1/(C9*D9)</f>
         <v>0.05</v>
       </c>
     </row>
@@ -1490,19 +1727,19 @@
       <c r="F10" s="17">
         <v>8.65</v>
       </c>
-      <c r="G10" s="30">
+      <c r="G10" s="29">
         <v>12.475</v>
       </c>
       <c r="H10" s="17">
         <v>14.6</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="29">
         <v>17.024999999999999</v>
       </c>
       <c r="J10" s="17">
         <v>20</v>
       </c>
-      <c r="K10" s="55">
+      <c r="K10" s="53">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1517,172 +1754,281 @@
       <c r="E11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <v>6.9666666666669999</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G11" s="29">
         <v>10.488888888889999</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="29">
         <v>13.02222222222</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="29">
         <v>14.78888888889</v>
       </c>
       <c r="J11" s="17">
         <v>20</v>
       </c>
-      <c r="K11" s="55">
+      <c r="K11" s="53">
         <f t="shared" si="0"/>
         <v>1.1111111111111112E-2</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C12" s="32">
+      <c r="C12" s="30">
         <v>5000</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="30">
         <v>0.01</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <v>10.72</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="30">
         <v>13.76</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="32">
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30">
         <v>20</v>
       </c>
-      <c r="K12" s="55">
+      <c r="K12" s="53">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C13" s="32">
+      <c r="C13" s="30">
         <v>5000</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="30">
         <v>0.02</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="55">
+      <c r="G13" s="30"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="53">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C14" s="32">
+      <c r="C14" s="30">
         <v>10000</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="30">
         <v>0.01</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="30">
         <v>10.77</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="55">
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="53">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C15" s="32">
+      <c r="C15" s="30">
         <v>10000</v>
       </c>
-      <c r="D15" s="32">
-        <v>0.02</v>
+      <c r="D15" s="30">
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="55">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C16" s="32">
-        <v>10000</v>
-      </c>
-      <c r="D16" s="32">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="30">
+      <c r="F15" s="29">
         <v>7.6177777777779996</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="55">
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="53">
         <f t="shared" si="0"/>
         <v>2.2222222222222222E-3</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C17" s="6">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C16" s="6">
         <v>10000</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D16" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F16" s="55">
         <v>7.3618181818180002</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="56">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="54">
         <f t="shared" si="0"/>
         <v>1.8181818181818182E-3</v>
       </c>
     </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C17" s="65">
+        <v>500</v>
+      </c>
+      <c r="D17" s="64">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="29">
+        <v>10.63716284146</v>
+      </c>
+      <c r="G17" s="29">
+        <v>14.02625857836</v>
+      </c>
+      <c r="H17" s="29">
+        <v>16.48710177809</v>
+      </c>
+      <c r="I17" s="29">
+        <v>18.139718386679998</v>
+      </c>
+      <c r="J17" s="65">
+        <v>20</v>
+      </c>
+      <c r="K17" s="53">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C18" s="32"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
+      <c r="C18" s="65">
+        <v>1000</v>
+      </c>
+      <c r="D18" s="64">
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="29">
+        <v>10.767489626570001</v>
+      </c>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="53">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="E19" s="1"/>
+      <c r="C19" s="65">
+        <v>500</v>
+      </c>
+      <c r="D19" s="64">
+        <v>0.02</v>
+      </c>
+      <c r="E19" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="29">
+        <v>8.9027781157889994</v>
+      </c>
+      <c r="G19" s="29"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="53">
+        <f t="shared" ref="K19:K21" si="1">1/(C19*D19)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C20" s="65">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="64">
+        <v>0.02</v>
+      </c>
+      <c r="E20" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="29">
+        <v>9.0248333085620001</v>
+      </c>
+      <c r="G20" s="29"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="53">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C21" s="65">
+        <v>2000</v>
+      </c>
+      <c r="D21" s="64">
+        <v>0.02</v>
+      </c>
+      <c r="E21" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="29">
+        <v>9.2639695601260001</v>
+      </c>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="53">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="53"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C23" s="30"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1696,7 +2042,7 @@
   <dimension ref="B2:S33"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1711,28 +2057,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="O2" s="63" t="s">
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="O2" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="11"/>
@@ -1784,7 +2130,7 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="73" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="22">
@@ -1809,7 +2155,7 @@
       <c r="J4" s="15">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="33">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="L4" s="15">
@@ -1835,7 +2181,7 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="68"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="20">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -1858,13 +2204,13 @@
       <c r="J5" s="13">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="33">
         <v>1.2E-2</v>
       </c>
       <c r="L5" s="13">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="M5" s="52">
+      <c r="M5" s="50">
         <v>0</v>
       </c>
       <c r="O5" s="20">
@@ -1884,7 +2230,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="20">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1907,13 +2253,13 @@
       <c r="J6" s="13">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="33">
         <v>2E-3</v>
       </c>
       <c r="L6" s="13">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="M6" s="52">
+      <c r="M6" s="50">
         <v>0</v>
       </c>
       <c r="O6" s="20">
@@ -1933,7 +2279,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="68"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="20">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -1956,13 +2302,13 @@
       <c r="J7" s="13">
         <v>1E-3</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="33">
         <v>4.4999999999999997E-3</v>
       </c>
       <c r="L7" s="13">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="M7" s="52">
+      <c r="M7" s="50">
         <v>0</v>
       </c>
       <c r="O7" s="20">
@@ -1982,7 +2328,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="68"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="20">
         <v>2.5000000000000001E-3</v>
       </c>
@@ -2005,13 +2351,13 @@
       <c r="J8" s="13">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="33">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="L8" s="13">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="50">
         <v>0</v>
       </c>
       <c r="O8" s="20">
@@ -2031,7 +2377,7 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="68"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="20">
         <v>4.4999999999999997E-3</v>
       </c>
@@ -2054,13 +2400,13 @@
       <c r="J9" s="13">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="33">
         <v>3.5000000000000001E-3</v>
       </c>
       <c r="L9" s="13">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="M9" s="52">
+      <c r="M9" s="50">
         <v>0</v>
       </c>
       <c r="O9" s="20"/>
@@ -2078,7 +2424,7 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="68"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="20">
         <v>3.5000000000000001E-3</v>
       </c>
@@ -2097,13 +2443,13 @@
       <c r="J10" s="13">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="33">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="L10" s="13">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="M10" s="52">
+      <c r="M10" s="50">
         <v>0</v>
       </c>
       <c r="O10" s="20"/>
@@ -2121,7 +2467,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="69"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="21"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24">
@@ -2134,7 +2480,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="35">
+      <c r="K11" s="33">
         <v>0.01</v>
       </c>
       <c r="L11" s="14">
@@ -2196,45 +2542,45 @@
         <f>MAX(M4:M11)</f>
         <v>0</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="35">
         <f>MAX(O4:O11)</f>
         <v>2.1499999999999998E-2</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="35">
         <f>MAX(P4:P11)</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Q12" s="37">
+      <c r="Q12" s="35">
         <f>MAX(Q4:Q11)</f>
         <v>2.7E-2</v>
       </c>
-      <c r="R12" s="37">
+      <c r="R12" s="35">
         <f>MAX(R4:R11)</f>
         <v>2.4500000000000001E-2</v>
       </c>
-      <c r="S12" s="37">
+      <c r="S12" s="35">
         <f>MAX(S4:S11)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:19" s="44" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="38"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
+    <row r="13" spans="2:19" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="36"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="18"/>
@@ -2286,372 +2632,372 @@
       </c>
     </row>
     <row r="15" spans="2:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="44">
         <v>6.0879999999999997E-3</v>
       </c>
-      <c r="D15" s="46">
+      <c r="D15" s="44">
         <v>3.7079999999999999E-3</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="44">
         <v>3.7699999999999999E-3</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="44">
         <v>3.6410000000000001E-3</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="44">
         <v>0</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="33">
+      <c r="I15" s="31">
         <v>5.8060000000000004E-3</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="31">
         <v>3.908E-3</v>
       </c>
-      <c r="K15" s="33">
+      <c r="K15" s="31">
         <v>5.5659999999999998E-3</v>
       </c>
-      <c r="L15" s="33">
+      <c r="L15" s="31">
         <v>8.685E-3</v>
       </c>
-      <c r="M15" s="33">
-        <v>0</v>
-      </c>
-      <c r="O15" s="46">
+      <c r="M15" s="31">
+        <v>0</v>
+      </c>
+      <c r="O15" s="44">
         <v>2.4768999999999999E-2</v>
       </c>
-      <c r="P15" s="46">
+      <c r="P15" s="44">
         <v>2.2866999999999998E-2</v>
       </c>
-      <c r="Q15" s="46">
+      <c r="Q15" s="44">
         <v>3.0321000000000001E-2</v>
       </c>
-      <c r="R15" s="46">
+      <c r="R15" s="44">
         <v>2.5621999999999999E-2</v>
       </c>
-      <c r="S15" s="46">
+      <c r="S15" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B16" s="68"/>
-      <c r="C16" s="47">
+      <c r="B16" s="74"/>
+      <c r="C16" s="45">
         <v>3.712E-3</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="45">
         <v>3.7590000000000002E-3</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="45">
         <v>3.7850000000000002E-3</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="45">
         <v>5.0650000000000001E-3</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="45">
         <v>0</v>
       </c>
       <c r="H16" s="13"/>
-      <c r="I16" s="49">
+      <c r="I16" s="47">
         <v>6.0150000000000004E-3</v>
       </c>
-      <c r="J16" s="49">
+      <c r="J16" s="47">
         <v>1.3932E-2</v>
       </c>
-      <c r="K16" s="34">
+      <c r="K16" s="32">
         <v>1.179E-2</v>
       </c>
-      <c r="L16" s="49">
+      <c r="L16" s="47">
         <v>8.7019999999999997E-3</v>
       </c>
-      <c r="M16" s="50">
-        <v>0</v>
-      </c>
-      <c r="O16" s="53">
+      <c r="M16" s="48">
+        <v>0</v>
+      </c>
+      <c r="O16" s="51">
         <v>2.4708999999999998E-2</v>
       </c>
-      <c r="P16" s="53">
+      <c r="P16" s="51">
         <v>1.1729E-2</v>
       </c>
-      <c r="Q16" s="53">
+      <c r="Q16" s="51">
         <v>3.0207000000000001E-2</v>
       </c>
-      <c r="R16" s="53">
+      <c r="R16" s="51">
         <v>9.8410000000000008E-3</v>
       </c>
-      <c r="S16" s="53">
+      <c r="S16" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B17" s="68"/>
-      <c r="C17" s="47">
+      <c r="B17" s="74"/>
+      <c r="C17" s="45">
         <v>3.6310000000000001E-3</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="45">
         <v>3.7320000000000001E-3</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="45">
         <v>3.8210000000000002E-3</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="45">
         <v>3.8119999999999999E-3</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="45">
         <v>0</v>
       </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="49">
+      <c r="I17" s="47">
         <v>5.973E-3</v>
       </c>
-      <c r="J17" s="49">
+      <c r="J17" s="47">
         <v>3.7910000000000001E-3</v>
       </c>
-      <c r="K17" s="34">
+      <c r="K17" s="32">
         <v>5.5849999999999997E-3</v>
       </c>
-      <c r="L17" s="49">
+      <c r="L17" s="47">
         <v>1.0119E-2</v>
       </c>
-      <c r="M17" s="50">
-        <v>0</v>
-      </c>
-      <c r="O17" s="53">
+      <c r="M17" s="48">
+        <v>0</v>
+      </c>
+      <c r="O17" s="51">
         <v>2.4674999999999999E-2</v>
       </c>
-      <c r="P17" s="53">
+      <c r="P17" s="51">
         <v>2.2794999999999999E-2</v>
       </c>
-      <c r="Q17" s="53">
+      <c r="Q17" s="51">
         <v>1.1520000000000001E-2</v>
       </c>
-      <c r="R17" s="53">
+      <c r="R17" s="51">
         <v>9.8250000000000004E-3</v>
       </c>
-      <c r="S17" s="53">
+      <c r="S17" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="68"/>
-      <c r="C18" s="47">
+      <c r="B18" s="74"/>
+      <c r="C18" s="45">
         <v>3.5200000000000001E-3</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="45">
         <v>3.738E-3</v>
       </c>
-      <c r="E18" s="47">
+      <c r="E18" s="45">
         <v>3.846E-3</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="45">
         <v>3.6779999999999998E-3</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="45">
         <v>0</v>
       </c>
       <c r="H18" s="13"/>
-      <c r="I18" s="49">
+      <c r="I18" s="47">
         <v>8.8610000000000008E-3</v>
       </c>
-      <c r="J18" s="49">
+      <c r="J18" s="47">
         <v>2.516E-3</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="32">
         <v>5.6779999999999999E-3</v>
       </c>
-      <c r="L18" s="49">
+      <c r="L18" s="47">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="M18" s="50">
-        <v>0</v>
-      </c>
-      <c r="O18" s="53">
+      <c r="M18" s="48">
+        <v>0</v>
+      </c>
+      <c r="O18" s="51">
         <v>2.4604000000000001E-2</v>
       </c>
-      <c r="P18" s="53">
+      <c r="P18" s="51">
         <v>2.2870999999999999E-2</v>
       </c>
-      <c r="Q18" s="53">
+      <c r="Q18" s="51">
         <v>3.0634999999999999E-2</v>
       </c>
-      <c r="R18" s="53">
+      <c r="R18" s="51">
         <v>9.9830000000000006E-3</v>
       </c>
-      <c r="S18" s="53">
+      <c r="S18" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B19" s="68"/>
-      <c r="C19" s="47">
+      <c r="B19" s="74"/>
+      <c r="C19" s="45">
         <v>6.0010000000000003E-3</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="45">
         <v>3.6770000000000001E-3</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="45">
         <v>5.4949999999999999E-3</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="45">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="45">
         <v>0</v>
       </c>
       <c r="H19" s="13"/>
-      <c r="I19" s="49">
+      <c r="I19" s="47">
         <v>8.9079999999999993E-3</v>
       </c>
-      <c r="J19" s="49">
+      <c r="J19" s="47">
         <v>2.5530000000000001E-3</v>
       </c>
-      <c r="K19" s="34">
+      <c r="K19" s="32">
         <v>1.184E-2</v>
       </c>
-      <c r="L19" s="49">
+      <c r="L19" s="47">
         <v>1.0104999999999999E-2</v>
       </c>
-      <c r="M19" s="50">
-        <v>0</v>
-      </c>
-      <c r="O19" s="53">
+      <c r="M19" s="48">
+        <v>0</v>
+      </c>
+      <c r="O19" s="51">
         <v>2.4759E-2</v>
       </c>
-      <c r="P19" s="53">
+      <c r="P19" s="51">
         <v>2.2712E-2</v>
       </c>
-      <c r="Q19" s="53">
+      <c r="Q19" s="51">
         <v>3.0180999999999999E-2</v>
       </c>
-      <c r="R19" s="53">
+      <c r="R19" s="51">
         <v>2.5248E-2</v>
       </c>
-      <c r="S19" s="53">
+      <c r="S19" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B20" s="68"/>
-      <c r="C20" s="47">
+      <c r="B20" s="74"/>
+      <c r="C20" s="45">
         <v>3.6089999999999998E-3</v>
       </c>
-      <c r="D20" s="47">
+      <c r="D20" s="45">
         <v>3.7859999999999999E-3</v>
       </c>
-      <c r="E20" s="47">
+      <c r="E20" s="45">
         <v>3.8089999999999999E-3</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="45">
         <v>3.5969999999999999E-3</v>
       </c>
-      <c r="G20" s="47">
+      <c r="G20" s="45">
         <v>0</v>
       </c>
       <c r="H20" s="13"/>
-      <c r="I20" s="49">
+      <c r="I20" s="47">
         <v>5.9750000000000003E-3</v>
       </c>
-      <c r="J20" s="49">
+      <c r="J20" s="47">
         <v>8.4229999999999999E-3</v>
       </c>
-      <c r="K20" s="34">
+      <c r="K20" s="32">
         <v>5.5240000000000003E-3</v>
       </c>
-      <c r="L20" s="49">
+      <c r="L20" s="47">
         <v>8.6149999999999994E-3</v>
       </c>
-      <c r="M20" s="50">
-        <v>0</v>
-      </c>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53">
+      <c r="M20" s="48">
+        <v>0</v>
+      </c>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51">
         <v>1.4152E-2</v>
       </c>
-      <c r="Q20" s="53">
+      <c r="Q20" s="51">
         <v>1.1768000000000001E-2</v>
       </c>
-      <c r="R20" s="53">
+      <c r="R20" s="51">
         <v>2.5838E-2</v>
       </c>
-      <c r="S20" s="53">
+      <c r="S20" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="68"/>
-      <c r="C21" s="47">
+      <c r="B21" s="74"/>
+      <c r="C21" s="45">
         <v>3.7139999999999999E-3</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47">
+      <c r="D21" s="45"/>
+      <c r="E21" s="45">
         <v>5.6709999999999998E-3</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47">
+      <c r="F21" s="45"/>
+      <c r="G21" s="45">
         <v>0</v>
       </c>
       <c r="H21" s="13"/>
-      <c r="I21" s="49">
+      <c r="I21" s="47">
         <v>8.7600000000000004E-3</v>
       </c>
-      <c r="J21" s="49">
+      <c r="J21" s="47">
         <v>8.2799999999999992E-3</v>
       </c>
-      <c r="K21" s="34">
+      <c r="K21" s="32">
         <v>1.1852E-2</v>
       </c>
-      <c r="L21" s="49">
+      <c r="L21" s="47">
         <v>8.5699999999999995E-3</v>
       </c>
-      <c r="M21" s="50">
-        <v>0</v>
-      </c>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53">
+      <c r="M21" s="48">
+        <v>0</v>
+      </c>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51">
         <v>1.4112E-2</v>
       </c>
-      <c r="Q21" s="53">
+      <c r="Q21" s="51">
         <v>1.1705999999999999E-2</v>
       </c>
-      <c r="R21" s="53">
+      <c r="R21" s="51">
         <v>1.0019999999999999E-2</v>
       </c>
-      <c r="S21" s="53">
+      <c r="S21" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="69"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48">
+      <c r="B22" s="75"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46">
         <v>3.777E-3</v>
       </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48">
+      <c r="F22" s="46"/>
+      <c r="G22" s="46">
         <v>0</v>
       </c>
       <c r="H22" s="14"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="34">
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="32">
         <v>1.1841000000000001E-2</v>
       </c>
-      <c r="L22" s="51">
+      <c r="L22" s="49">
         <v>8.4989999999999996E-3</v>
       </c>
-      <c r="M22" s="51">
-        <v>0</v>
-      </c>
-      <c r="O22" s="53"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="53">
+      <c r="M22" s="49">
+        <v>0</v>
+      </c>
+      <c r="O22" s="51"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51">
         <v>2.5666999999999999E-2</v>
       </c>
-      <c r="S22" s="53">
+      <c r="S22" s="51">
         <v>0</v>
       </c>
     </row>
@@ -2698,48 +3044,48 @@
         <f>MAX(M15:M22)</f>
         <v>0</v>
       </c>
-      <c r="O23" s="36">
+      <c r="O23" s="34">
         <f>MAX(O15:O22)</f>
         <v>2.4768999999999999E-2</v>
       </c>
-      <c r="P23" s="36">
+      <c r="P23" s="34">
         <f>MAX(P15:P22)</f>
         <v>2.2870999999999999E-2</v>
       </c>
-      <c r="Q23" s="36">
+      <c r="Q23" s="34">
         <f>MAX(Q15:Q22)</f>
         <v>3.0634999999999999E-2</v>
       </c>
-      <c r="R23" s="36">
+      <c r="R23" s="34">
         <f>MAX(R15:R22)</f>
         <v>2.5838E-2</v>
       </c>
-      <c r="S23" s="36">
+      <c r="S23" s="34">
         <f>MAX(S15:S22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:19" s="60" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="61"/>
+    <row r="24" spans="2:19" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="57"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="59"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="68" t="s">
         <v>28</v>
       </c>
       <c r="C25">
@@ -2747,46 +3093,46 @@
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B26" s="62"/>
+      <c r="B26" s="68"/>
       <c r="C26">
         <v>2.25</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="62"/>
+      <c r="B27" s="68"/>
       <c r="C27">
         <v>1.35</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B28" s="62"/>
+      <c r="B28" s="68"/>
       <c r="C28">
         <v>1.35</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B29" s="62"/>
+      <c r="B29" s="68"/>
       <c r="C29">
         <v>1.25</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B30" s="62"/>
+      <c r="B30" s="68"/>
       <c r="C30">
         <v>1.45</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B31" s="62"/>
+      <c r="B31" s="68"/>
       <c r="C31">
         <v>1.35</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B32" s="62"/>
+      <c r="B32" s="68"/>
     </row>
     <row r="33" spans="2:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="56" t="s">
         <v>27</v>
       </c>
       <c r="C33">
@@ -2810,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2837,7 +3183,7 @@
       <c r="G5" s="27"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="73" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="22">
@@ -2851,7 +3197,7 @@
       <c r="G6" s="22"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="68"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="20">
         <v>2.5999999999999999E-3</v>
       </c>
@@ -2863,7 +3209,7 @@
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="68"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="20">
         <v>5.4000000000000003E-3</v>
       </c>
@@ -2875,7 +3221,7 @@
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="68"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="20">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -2887,7 +3233,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="68"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="20">
         <v>2E-3</v>
       </c>
@@ -2899,7 +3245,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="68"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="20">
         <v>3.8E-3</v>
       </c>
@@ -2911,7 +3257,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="68"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="20">
         <v>5.5999999999999999E-3</v>
       </c>
@@ -2923,7 +3269,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="69"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="21"/>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
@@ -2954,12 +3300,12 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="38"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="18"/>
@@ -2974,98 +3320,98 @@
       <c r="G16" s="27"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="71">
+      <c r="C17" s="60">
         <v>3.5760000000000002E-3</v>
       </c>
-      <c r="D17" s="71">
+      <c r="D17" s="60">
         <v>8.8310000000000003E-3</v>
       </c>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="68"/>
-      <c r="C18" s="72">
+      <c r="B18" s="74"/>
+      <c r="C18" s="61">
         <v>3.6180000000000001E-3</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="61">
         <v>6.0219999999999996E-3</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="68"/>
-      <c r="C19" s="72">
+      <c r="B19" s="74"/>
+      <c r="C19" s="61">
         <v>5.8820000000000001E-3</v>
       </c>
-      <c r="D19" s="72">
+      <c r="D19" s="61">
         <v>5.9160000000000003E-3</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="68"/>
-      <c r="C20" s="72">
+      <c r="B20" s="74"/>
+      <c r="C20" s="61">
         <v>3.4480000000000001E-3</v>
       </c>
-      <c r="D20" s="72">
+      <c r="D20" s="61">
         <v>8.7889999999999999E-3</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="68"/>
-      <c r="C21" s="72">
+      <c r="B21" s="74"/>
+      <c r="C21" s="61">
         <v>3.7139999999999999E-3</v>
       </c>
-      <c r="D21" s="72">
+      <c r="D21" s="61">
         <v>5.8650000000000004E-3</v>
       </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="68"/>
-      <c r="C22" s="72">
+      <c r="B22" s="74"/>
+      <c r="C22" s="61">
         <v>3.5799999999999998E-3</v>
       </c>
-      <c r="D22" s="72">
+      <c r="D22" s="61">
         <v>5.9540000000000001E-3</v>
       </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="68"/>
-      <c r="C23" s="72">
+      <c r="B23" s="74"/>
+      <c r="C23" s="61">
         <v>5.8399999999999997E-3</v>
       </c>
-      <c r="D23" s="72">
+      <c r="D23" s="61">
         <v>8.8050000000000003E-3</v>
       </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="69"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
@@ -3091,7 +3437,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C27">
@@ -3102,7 +3448,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="70"/>
+      <c r="B28" s="76"/>
       <c r="C28">
         <v>1.26</v>
       </c>
@@ -3111,7 +3457,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="70"/>
+      <c r="B29" s="76"/>
       <c r="C29">
         <v>1.6</v>
       </c>
@@ -3120,7 +3466,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="70"/>
+      <c r="B30" s="76"/>
       <c r="C30">
         <v>1.4</v>
       </c>
@@ -3129,7 +3475,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="70"/>
+      <c r="B31" s="76"/>
       <c r="C31">
         <v>2.2000000000000002</v>
       </c>
@@ -3138,7 +3484,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="70"/>
+      <c r="B32" s="76"/>
       <c r="C32">
         <v>1.4</v>
       </c>
@@ -3147,7 +3493,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="70"/>
+      <c r="B33" s="76"/>
       <c r="C33">
         <v>1.58</v>
       </c>
@@ -3156,7 +3502,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="56" t="s">
         <v>27</v>
       </c>
       <c r="C34">
@@ -3180,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3211,7 +3557,7 @@
       <c r="G4" s="27"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="73" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="22">
@@ -3227,7 +3573,7 @@
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="68"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="20">
         <v>1.5E-3</v>
       </c>
@@ -3241,7 +3587,7 @@
       <c r="G6" s="20"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="68"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
@@ -3255,7 +3601,7 @@
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="68"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -3269,7 +3615,7 @@
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="68"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="20">
         <v>1.4E-3</v>
       </c>
@@ -3283,7 +3629,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="68"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20">
@@ -3295,7 +3641,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="68"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20">
@@ -3305,7 +3651,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="69"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="21"/>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
@@ -3336,12 +3682,12 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="38"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
@@ -3360,106 +3706,106 @@
       <c r="G15" s="27"/>
     </row>
     <row r="16" spans="2:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="73" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="22">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46">
+      <c r="D16" s="44"/>
+      <c r="E16" s="44">
         <v>1.2156E-2</v>
       </c>
-      <c r="F16" s="46">
+      <c r="F16" s="44">
         <v>1.1986E-2</v>
       </c>
-      <c r="G16" s="46"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="68"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47">
+      <c r="D17" s="45"/>
+      <c r="E17" s="45">
         <v>1.2014E-2</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="45">
         <v>1.2148000000000001E-2</v>
       </c>
-      <c r="G17" s="47"/>
+      <c r="G17" s="45"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="68"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="20">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47">
+      <c r="D18" s="45"/>
+      <c r="E18" s="45">
         <v>1.2083999999999999E-2</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="45">
         <v>1.2278000000000001E-2</v>
       </c>
-      <c r="G18" s="47"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="68"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="20">
         <v>1.4E-3</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47">
+      <c r="D19" s="45"/>
+      <c r="E19" s="45">
         <v>1.2336E-2</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="45">
         <v>1.1924000000000001E-2</v>
       </c>
-      <c r="G19" s="47"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="68"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47">
+      <c r="D20" s="45"/>
+      <c r="E20" s="45">
         <v>1.2062E-2</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="45">
         <v>1.1938000000000001E-2</v>
       </c>
-      <c r="G20" s="47"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="68"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47">
+      <c r="B21" s="74"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45">
         <v>1.2290000000000001E-2</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="45">
         <v>1.1885E-2</v>
       </c>
-      <c r="G21" s="47"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="68"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47">
+      <c r="B22" s="74"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45">
         <v>1.2336E-2</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="69"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="10"/>
@@ -3485,7 +3831,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="76" t="s">
         <v>28</v>
       </c>
       <c r="E26">
@@ -3496,7 +3842,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="70"/>
+      <c r="B27" s="76"/>
       <c r="E27">
         <v>1.2533300000000001</v>
       </c>
@@ -3505,7 +3851,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="70"/>
+      <c r="B28" s="76"/>
       <c r="E28">
         <v>1.28</v>
       </c>
@@ -3514,7 +3860,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="70"/>
+      <c r="B29" s="76"/>
       <c r="E29">
         <v>1.22444</v>
       </c>
@@ -3523,7 +3869,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="70"/>
+      <c r="B30" s="76"/>
       <c r="E30">
         <v>1.26</v>
       </c>
@@ -3532,7 +3878,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="70"/>
+      <c r="B31" s="76"/>
       <c r="E31">
         <v>1.2888900000000001</v>
       </c>
@@ -3541,10 +3887,10 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="70"/>
+      <c r="B32" s="76"/>
     </row>
     <row r="33" spans="2:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="56" t="s">
         <v>27</v>
       </c>
       <c r="E33">
@@ -3592,13 +3938,13 @@
       </c>
     </row>
     <row r="2" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C3" s="11"/>
@@ -3619,7 +3965,7 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="73" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="22">
@@ -3639,7 +3985,7 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C5" s="68"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="20">
         <v>1.5E-3</v>
       </c>
@@ -3657,7 +4003,7 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C6" s="68"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="20">
         <v>1.2999999999999999E-3</v>
       </c>
@@ -3675,7 +4021,7 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="68"/>
+      <c r="C7" s="74"/>
       <c r="D7" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -3693,7 +4039,7 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C8" s="68"/>
+      <c r="C8" s="74"/>
       <c r="D8" s="20">
         <v>1.4E-3</v>
       </c>
@@ -3711,7 +4057,7 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="68"/>
+      <c r="C9" s="74"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23">
         <v>2.2000000000000001E-3</v>
@@ -3727,7 +4073,7 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="68"/>
+      <c r="C10" s="74"/>
       <c r="D10" s="20"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23">
@@ -3739,7 +4085,7 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="69"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="21"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24">
@@ -3792,7 +4138,7 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="73" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="22">
@@ -3812,7 +4158,7 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="68"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="20">
         <v>1.6999999999999999E-3</v>
       </c>
@@ -3830,7 +4176,7 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="68"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="20">
         <v>1.6000000000000001E-3</v>
       </c>
@@ -3848,7 +4194,7 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C17" s="68"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="20">
         <v>1.4E-3</v>
       </c>
@@ -3866,7 +4212,7 @@
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C18" s="68"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="20">
         <v>2.2000000000000001E-3</v>
       </c>
@@ -3884,7 +4230,7 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C19" s="68"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23">
         <v>3.7829999999999999E-3</v>
@@ -3900,7 +4246,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C20" s="68"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="20"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23">
@@ -3912,7 +4258,7 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C21" s="69"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="21"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24">

</xml_diff>